<commit_message>
verigen : interface:signal_count() 추가, 단일 신호 bared signal 일 경우 interface_i 의 이름이 시그널 이름으로 갱신 됨.
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_interface.xlsx
+++ b/Common/doc/verigen/media/instruction_interface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F46BE8-BDBB-4D9A-9029-2D83FEFD9A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0EE216-02D2-4E65-9CF2-D746C5DF84A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="18390" windowHeight="15300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -22,17 +22,18 @@
     <sheet name="set_clock" sheetId="11" r:id="rId7"/>
     <sheet name="get_clock" sheetId="12" r:id="rId8"/>
     <sheet name="set_signal" sheetId="13" r:id="rId9"/>
-    <sheet name="set_param" sheetId="14" r:id="rId10"/>
-    <sheet name="get_param" sheetId="15" r:id="rId11"/>
-    <sheet name="set_modport" sheetId="16" r:id="rId12"/>
-    <sheet name="add_modport" sheetId="17" r:id="rId13"/>
-    <sheet name="get_modport" sheetId="18" r:id="rId14"/>
-    <sheet name="set_prefix" sheetId="19" r:id="rId15"/>
-    <sheet name="set_bared" sheetId="20" r:id="rId16"/>
-    <sheet name="i_set_port" sheetId="21" r:id="rId17"/>
-    <sheet name="i_set_desc" sheetId="22" r:id="rId18"/>
-    <sheet name="i_set_prefix" sheetId="23" r:id="rId19"/>
-    <sheet name="i_get_prefix" sheetId="24" r:id="rId20"/>
+    <sheet name="signal_count" sheetId="25" r:id="rId10"/>
+    <sheet name="set_param" sheetId="14" r:id="rId11"/>
+    <sheet name="get_param" sheetId="15" r:id="rId12"/>
+    <sheet name="set_modport" sheetId="16" r:id="rId13"/>
+    <sheet name="add_modport" sheetId="17" r:id="rId14"/>
+    <sheet name="get_modport" sheetId="18" r:id="rId15"/>
+    <sheet name="set_prefix" sheetId="19" r:id="rId16"/>
+    <sheet name="set_bared" sheetId="20" r:id="rId17"/>
+    <sheet name="i_set_port" sheetId="21" r:id="rId18"/>
+    <sheet name="i_set_desc" sheetId="22" r:id="rId19"/>
+    <sheet name="i_set_prefix" sheetId="23" r:id="rId20"/>
+    <sheet name="i_get_prefix" sheetId="24" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="120">
   <si>
     <t>clock</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -518,6 +519,26 @@
   </si>
   <si>
     <t>:get_prefix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:signal_count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신호 개수 얻기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function interface:signal_count()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interface에 정의된 signal 개수를 반환합니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -853,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -966,78 +987,89 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1049,6 +1081,56 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4847C089-FBC5-4B8A-B99B-9C9142BC36D8}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D19B922-7931-4B59-9944-8B3AC4588909}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1117,7 +1199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB79548-8FC2-4922-9FA9-03D11B2C5106}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1178,7 +1260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5AC875-2922-4564-962E-ED0096C28F9E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1247,7 +1329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D60330-BA3B-4597-B119-0C80BCDA160E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1308,7 +1390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BFA84B-9523-4CAC-A4BD-7D16A6BD030B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1361,7 +1443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6114427-72D5-4122-9DFD-3550749AF4EA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1414,7 +1496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CEA95C-E8AA-47A5-93A8-AEB05B2180E4}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1467,7 +1549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F2F3AF-FDE1-4836-8803-E97194A35FA4}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1520,7 +1602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C24CC8-12AA-4601-ABF2-E60277D812CD}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1573,7 +1655,69 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A76216-2298-479D-87E6-5C639887A995}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="3" max="3" width="33.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E34A79-A19B-4D4B-9395-FFCCB8C6B49F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1626,69 +1770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A76216-2298-479D-87E6-5C639887A995}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="33.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8558BD0-6E49-413F-8F7E-AE92B85712A2}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2097,7 +2179,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
verigen : interface:set_top_uppercase 함수 추가
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_interface.xlsx
+++ b/Common/doc/verigen/media/instruction_interface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0EE216-02D2-4E65-9CF2-D746C5DF84A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EC1737-D750-43E5-A4E7-244335436BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -30,10 +30,11 @@
     <sheet name="get_modport" sheetId="18" r:id="rId15"/>
     <sheet name="set_prefix" sheetId="19" r:id="rId16"/>
     <sheet name="set_bared" sheetId="20" r:id="rId17"/>
-    <sheet name="i_set_port" sheetId="21" r:id="rId18"/>
-    <sheet name="i_set_desc" sheetId="22" r:id="rId19"/>
-    <sheet name="i_set_prefix" sheetId="23" r:id="rId20"/>
-    <sheet name="i_get_prefix" sheetId="24" r:id="rId21"/>
+    <sheet name="set_top_uppercase" sheetId="26" r:id="rId18"/>
+    <sheet name="i_set_port" sheetId="21" r:id="rId19"/>
+    <sheet name="i_set_desc" sheetId="22" r:id="rId20"/>
+    <sheet name="i_set_prefix" sheetId="23" r:id="rId21"/>
+    <sheet name="i_get_prefix" sheetId="24" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="124">
   <si>
     <t>clock</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -539,6 +540,22 @@
   </si>
   <si>
     <t>interface에 정의된 signal 개수를 반환합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function interface:set_top_uppercase(en)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>en</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uppercase 여부, true(uppercase), false(lowercase), nil(원본)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interface 의 top 의 port 출력시 강제 대문자 또는 소문자 이름으로 강제합니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1084,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4847C089-FBC5-4B8A-B99B-9C9142BC36D8}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1550,6 +1567,59 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE109BF-A3BC-40C0-94F7-1CD099028E2F}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F2F3AF-FDE1-4836-8803-E97194A35FA4}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1602,7 +1672,69 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A76216-2298-479D-87E6-5C639887A995}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="3" max="3" width="33.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C24CC8-12AA-4601-ABF2-E60277D812CD}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1655,69 +1787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A76216-2298-479D-87E6-5C639887A995}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="33.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E34A79-A19B-4D4B-9395-FFCCB8C6B49F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1770,7 +1840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8558BD0-6E49-413F-8F7E-AE92B85712A2}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
verigen : Combines set_modport/add_modport functions into one and extends functionality.
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_interface.xlsx
+++ b/Common/doc/verigen/media/instruction_interface.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63672273-CC41-4DB9-9A11-32A42E27EB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A98AEFF-61FE-4DEC-837A-4257B5FFF382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="705" windowWidth="25725" windowHeight="15285" firstSheet="14" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -26,15 +26,14 @@
     <sheet name="set_param" sheetId="14" r:id="rId11"/>
     <sheet name="get_param" sheetId="15" r:id="rId12"/>
     <sheet name="set_modport" sheetId="16" r:id="rId13"/>
-    <sheet name="add_modport" sheetId="17" r:id="rId14"/>
-    <sheet name="get_modport" sheetId="18" r:id="rId15"/>
-    <sheet name="set_prefix" sheetId="19" r:id="rId16"/>
-    <sheet name="set_bared" sheetId="20" r:id="rId17"/>
-    <sheet name="set_top_uppercase" sheetId="26" r:id="rId18"/>
-    <sheet name="i_set_port" sheetId="21" r:id="rId19"/>
-    <sheet name="i_set_desc" sheetId="22" r:id="rId20"/>
-    <sheet name="i_set_prefix" sheetId="23" r:id="rId21"/>
-    <sheet name="i_get_prefix" sheetId="24" r:id="rId22"/>
+    <sheet name="get_modport" sheetId="18" r:id="rId14"/>
+    <sheet name="set_prefix" sheetId="19" r:id="rId15"/>
+    <sheet name="set_bared" sheetId="20" r:id="rId16"/>
+    <sheet name="set_top_uppercase" sheetId="26" r:id="rId17"/>
+    <sheet name="i_set_port" sheetId="21" r:id="rId18"/>
+    <sheet name="i_set_desc" sheetId="22" r:id="rId19"/>
+    <sheet name="i_set_prefix" sheetId="23" r:id="rId20"/>
+    <sheet name="i_get_prefix" sheetId="24" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="121">
   <si>
     <t>clock</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -224,10 +223,6 @@
   </si>
   <si>
     <t>modport</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>function interface:add_modport(name, modport)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -482,20 +477,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Add modport to interface.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>modport name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>It is a modport configuration table structure, and is described in the form below.
-{["input"]={"", ...}, ["output"]={"", ...}, ["inout"]={"", ...}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adds a signal to an existing modport of an interface.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -546,6 +528,23 @@
   </si>
   <si>
     <t>Returns the prefix of the interface instance added with the module:add_interface function. If no prefix is specified in the interface instance, the prefix of the original interface is returned.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add/Remove modport to interface.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modport name, or set dual mirrored modport with 'normal_name/inverted_name'
+ex) 'm' and 's' modport is exactly mirrored.
+     set_modport("m", m_~) set_modport('s', s_~)
+     = set_modport("m/s", m_~)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>It is a modport configuration table structure, and is described in the form below. If modport is nil, modport as 'name' will be lost all I/O signal list.
+add : {["input"]={"", ...}, ["output"]={"", ...}, ["inout"]={"", ...}}
+remove : {["-input"]={"", ...}, ["-output"]={"", ...}, ["-inout"]={"", ...}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -912,7 +911,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -923,7 +922,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -934,7 +933,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -945,7 +944,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -956,7 +955,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -967,7 +966,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -978,7 +977,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -989,18 +988,18 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1011,7 +1010,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1022,7 +1021,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1033,7 +1032,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1044,7 +1043,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1055,7 +1054,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1066,7 +1065,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1077,7 +1076,7 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1111,26 +1110,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1164,7 +1163,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
@@ -1172,7 +1171,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1180,10 +1179,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1191,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1199,7 +1198,7 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1233,7 +1232,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1241,18 +1240,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1260,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1274,9 +1273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5AC875-2922-4564-962E-ED0096C28F9E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B15:B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1294,7 +1291,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
@@ -1302,7 +1299,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1310,26 +1307,26 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1340,75 +1337,6 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D60330-BA3B-4597-B119-0C80BCDA160E}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="55.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BFA84B-9523-4CAC-A4BD-7D16A6BD030B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1432,26 +1360,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1459,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1469,7 +1397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6114427-72D5-4122-9DFD-3550749AF4EA}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1493,15 +1421,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1509,18 +1437,18 @@
     </row>
     <row r="4" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1530,7 +1458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CEA95C-E8AA-47A5-93A8-AEB05B2180E4}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1554,15 +1482,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1570,18 +1498,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1591,7 +1519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE109BF-A3BC-40C0-94F7-1CD099028E2F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1615,15 +1543,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1631,18 +1559,18 @@
     </row>
     <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1652,7 +1580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F2F3AF-FDE1-4836-8803-E97194A35FA4}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1676,15 +1604,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1692,18 +1620,79 @@
     </row>
     <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C24CC8-12AA-4601-ABF2-E60277D812CD}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
         <v>50</v>
       </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1740,24 +1729,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1768,18 +1757,18 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1789,67 +1778,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C24CC8-12AA-4601-ABF2-E60277D812CD}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="55.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E34A79-A19B-4D4B-9395-FFCCB8C6B49F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1873,15 +1801,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1889,18 +1817,18 @@
     </row>
     <row r="4" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1910,11 +1838,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8558BD0-6E49-413F-8F7E-AE92B85712A2}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1932,15 +1860,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1948,10 +1876,10 @@
     </row>
     <row r="4" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1984,7 +1912,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -1992,7 +1920,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2000,10 +1928,10 @@
     </row>
     <row r="4" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2011,7 +1939,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2045,7 +1973,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
@@ -2053,7 +1981,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2061,10 +1989,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2072,7 +2000,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2080,7 +2008,7 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2113,7 +2041,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -2121,7 +2049,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2129,10 +2057,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2140,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2173,7 +2101,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
@@ -2181,7 +2109,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -2189,10 +2117,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2200,7 +2128,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2233,7 +2161,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -2241,7 +2169,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -2249,10 +2177,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2260,7 +2188,7 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2294,7 +2222,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -2302,7 +2230,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2310,10 +2238,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2346,7 +2274,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -2354,7 +2282,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -2362,10 +2290,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2373,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2381,7 +2309,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>